<commit_message>
dsnvel: new version(search function)
</commit_message>
<xml_diff>
--- a/hih2023/data/example.xlsx
+++ b/hih2023/data/example.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan\Desktop\hih2023_junior\hih2023\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danil\Desktop\Hacaton\hih2023_junior\hih2023\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923E32F5-149C-465D-8FED-43DC80BBFF80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{440A67D6-57CC-4A35-812F-91ACA903AEB9}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -138,7 +137,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -169,9 +168,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -485,267 +495,277 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{855432CD-0E0C-4D67-BC23-51CBC73AF075}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
     <col min="5" max="5" width="12.21875" customWidth="1"/>
     <col min="6" max="6" width="13.44140625" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:7" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>44187</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="2">
         <v>44562</v>
       </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>33963</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="2">
         <v>33970</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>375</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>45198</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="2">
         <v>45200</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>1670</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>45209</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="2">
         <v>45231</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>45069</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="2">
         <v>45108</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="4">
         <v>43442</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
         <v>43328</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="2">
         <v>43466</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
         <v>42575</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="2">
         <v>42583</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>475</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="2">
         <v>44919</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="2">
         <v>44927</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>18</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="2">
         <v>45050</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="2">
         <v>45078</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>336</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="2">
         <v>44988</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="2">
         <v>45017</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="2">
         <v>45153</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="2">
         <v>45170</v>
       </c>
+      <c r="G12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
dsnvel: add function to search matches in filenames
</commit_message>
<xml_diff>
--- a/hih2023/data/example.xlsx
+++ b/hih2023/data/example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="1764" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -496,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection sqref="A1:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,6 +767,16 @@
       </c>
       <c r="G12" s="1"/>
     </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>